<commit_message>
Backup QR Scanner data - 2025-12-18T04:15:57.997Z - Cache Bust: 1766031357997
</commit_message>
<xml_diff>
--- a/log_history/Y3_B2526_Anatomy_scanner1765952358665_d32a41f0edf027fbaba50a548472bb628aaf9f0745a69b0f7306d7205f001922.xlsx
+++ b/log_history/Y3_B2526_Anatomy_scanner1765952358665_d32a41f0edf027fbaba50a548472bb628aaf9f0745a69b0f7306d7205f001922.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Anatomy" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1142,9 +1142,789 @@
         <v>nahla.nagiub@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>234612</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C38" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D38" t="str">
+        <v>10:21:53</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F38" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>234302</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C39" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D39" t="str">
+        <v>10:21:56</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F39" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>234751</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C40" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D40" t="str">
+        <v>10:21:59</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F40" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>234314</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C41" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D41" t="str">
+        <v>10:22:01</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F41" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>234609</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C42" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D42" t="str">
+        <v>10:22:04</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F42" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>234319</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C43" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D43" t="str">
+        <v>10:22:06</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F43" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>234281</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C44" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D44" t="str">
+        <v>10:22:09</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F44" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>234271</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C45" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D45" t="str">
+        <v>10:22:11</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F45" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>234316</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C46" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D46" t="str">
+        <v>10:22:14</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F46" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>234313</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C47" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D47" t="str">
+        <v>10:22:17</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F47" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>234330</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C48" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D48" t="str">
+        <v>10:22:20</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F48" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>234361</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C49" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D49" t="str">
+        <v>10:22:23</v>
+      </c>
+      <c r="E49" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F49" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>234365</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C50" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D50" t="str">
+        <v>10:22:25</v>
+      </c>
+      <c r="E50" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F50" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>234362</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C51" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D51" t="str">
+        <v>10:22:28</v>
+      </c>
+      <c r="E51" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F51" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>234194</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C52" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D52" t="str">
+        <v>10:22:33</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F52" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>234221</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C53" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D53" t="str">
+        <v>10:22:35</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F53" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>234260</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C54" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D54" t="str">
+        <v>10:22:38</v>
+      </c>
+      <c r="E54" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F54" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>234480</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C55" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D55" t="str">
+        <v>10:22:39</v>
+      </c>
+      <c r="E55" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F55" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>234317</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C56" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D56" t="str">
+        <v>10:22:40</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F56" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>234259</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C57" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D57" t="str">
+        <v>10:22:47</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F57" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>234284</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C58" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D58" t="str">
+        <v>10:22:50</v>
+      </c>
+      <c r="E58" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F58" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>234198</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C59" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D59" t="str">
+        <v>10:38:34</v>
+      </c>
+      <c r="E59" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F59" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>234199</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C60" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D60" t="str">
+        <v>10:38:37</v>
+      </c>
+      <c r="E60" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F60" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>234441</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C61" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D61" t="str">
+        <v>10:53:31</v>
+      </c>
+      <c r="E61" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F61" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>234176</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C62" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D62" t="str">
+        <v>10:53:35</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F62" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>234607</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C63" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D63" t="str">
+        <v>10:53:54</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F63" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>234294</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C64" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D64" t="str">
+        <v>10:54:02</v>
+      </c>
+      <c r="E64" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F64" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>234878</v>
+      </c>
+      <c r="B65" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C65" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D65" t="str">
+        <v>10:54:12</v>
+      </c>
+      <c r="E65" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F65" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>234246</v>
+      </c>
+      <c r="B66" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C66" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D66" t="str">
+        <v>10:54:32</v>
+      </c>
+      <c r="E66" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F66" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>234293</v>
+      </c>
+      <c r="B67" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C67" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D67" t="str">
+        <v>10:54:41</v>
+      </c>
+      <c r="E67" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F67" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>234382</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C68" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D68" t="str">
+        <v>10:55:06</v>
+      </c>
+      <c r="E68" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F68" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>234389</v>
+      </c>
+      <c r="B69" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C69" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D69" t="str">
+        <v>10:55:21</v>
+      </c>
+      <c r="E69" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F69" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>234522</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C70" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D70" t="str">
+        <v>10:55:28</v>
+      </c>
+      <c r="E70" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F70" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>234508</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C71" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D71" t="str">
+        <v>10:55:36</v>
+      </c>
+      <c r="E71" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F71" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>234523</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C72" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D72" t="str">
+        <v>10:55:44</v>
+      </c>
+      <c r="E72" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F72" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>234277</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C73" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D73" t="str">
+        <v>10:56:10</v>
+      </c>
+      <c r="E73" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F73" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>231068</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C74" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D74" t="str">
+        <v>10:56:18</v>
+      </c>
+      <c r="E74" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F74" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>234286</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C75" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D75" t="str">
+        <v>10:56:30</v>
+      </c>
+      <c r="E75" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F75" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>234266</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C76" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D76" t="str">
+        <v>10:56:42</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F76" t="str">
+        <v>nahla.nagiub@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F37"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F76"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>